<commit_message>
Khao sat website bán hang
</commit_message>
<xml_diff>
--- a/BangKeHoach-DoAn1.xlsx
+++ b/BangKeHoach-DoAn1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>DANH SÁCH CÔNG VIỆC</t>
   </si>
@@ -40,12 +40,6 @@
   </si>
   <si>
     <t>…</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn A</t>
-  </si>
-  <si>
-    <t>Trần Thị B</t>
   </si>
   <si>
     <t>Khảo sát A</t>
@@ -73,6 +67,52 @@
   </si>
   <si>
     <t>Đề tài: Web quản lý bán hàng online</t>
+  </si>
+  <si>
+    <t>Trần Văn Tuấn</t>
+  </si>
+  <si>
+    <t>Đoàn Văn Đức</t>
+  </si>
+  <si>
+    <t>7/102019</t>
+  </si>
+  <si>
+    <t>Khảo sát website bán hàng tiki.vn
+Ưu điểm: 
++ tốc độ load trang nhanh.
++ Dễ dàng tìm kiếm sản phẩm.
++ Có responsive web phù hợp trên mọi thiết bị.
++ Có phần tải app cho mobile trên trang.
++ Có hỗ trợ các phương thức thanh toán online qua nhiều loại thẻ tín dụng ATM.
++ Có cổng kết nối với các kênh youtube, facebook, zalo.
+Có hỗ trợ các phương thước login với tài khoản xã hội tin cậy facebook, zalo, google.
++ Dễ tìm kiếm sản phầm theo mức giá theo yêu cầu của người dùng.
++ Hỗ trợ dịch vụ đối với điện thoại.
++ Thanh tìm kiếm có hộ trợ từ khóa tìm kiếm nhanh.
+Nhược điểm:
++ Không hỗ trợ chat trược tuyến trên web.
++ nhiều thông tin trên một trang quá.
++ Dàn trải loyout trên trang quá nhiều, gây rỗi.</t>
+  </si>
+  <si>
+    <t>Khảo sát website bán hàng lazada.vn
+Ưu điểm: 
+ + Có hỗ trợ đa ngôn ngữ
+ + Cho phép tìm kiếm theo các từ khóa được tìm nhiều nhất.
+Nhược điểm:
+ + Thiết kế cực kì rườm rà không thích mắt.
+ + Không hiểu thị các tìm kiếm cũ.
+ + không hỗ trợ giữ chế độ đăng nhập.</t>
+  </si>
+  <si>
+    <t>kháo sát website bán hàng fptshop.com.vn
+Ưu điểm:
+ + Thiết kế phù hợp với thời đại.
+ + Sản phẩm được phân vùng hiển thị hợp lý.
+Nhước điểm:
+ + Trang không cho phép đăng nhập hay tạo tài khoản nên khi reload trình duyệt sẽ mất các sản phẩm dự định mua trong giỏ.
+ + Trang cũng không hỗ trợ chatbot hay hỗ trợ trực tuyến.</t>
   </si>
 </sst>
 </file>
@@ -230,6 +270,142 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2819400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1238250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect r="21755"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2009775" y="2847975"/>
+          <a:ext cx="2695575" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>207804</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2781300</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1285875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1981199" y="8046879"/>
+          <a:ext cx="2686051" cy="1078071"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>231182</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2895600</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1247775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1990724" y="11003957"/>
+          <a:ext cx="2790826" cy="1016593"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -529,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1001"/>
+  <dimension ref="A1:W1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -547,7 +723,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -574,7 +750,7 @@
     </row>
     <row r="2" spans="1:23" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -607,10 +783,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>2</v>
@@ -642,7 +818,7 @@
     </row>
     <row r="4" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
@@ -669,10 +845,10 @@
     </row>
     <row r="5" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="7">
@@ -701,11 +877,11 @@
     </row>
     <row r="6" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6" s="7">
         <v>43713</v>
@@ -733,11 +909,11 @@
     </row>
     <row r="7" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E7" s="7">
         <v>43722</v>
@@ -765,10 +941,10 @@
     </row>
     <row r="8" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="7">
@@ -795,17 +971,26 @@
       <c r="V8" s="8"/>
       <c r="W8" s="8"/>
     </row>
-    <row r="9" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>16</v>
+    <row r="9" spans="1:23" s="16" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>19</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
+      <c r="C9" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="D9" s="10"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="E9" s="7">
+        <v>43745</v>
+      </c>
+      <c r="F9" s="7">
+        <v>43745</v>
+      </c>
+      <c r="G9" s="7">
+        <v>43745</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -822,24 +1007,26 @@
       <c r="V9" s="8"/>
       <c r="W9" s="8"/>
     </row>
-    <row r="10" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" s="16" customFormat="1" ht="231" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>14</v>
-      </c>
+      <c r="D10" s="10"/>
       <c r="E10" s="7">
-        <v>43728</v>
+        <v>43747</v>
       </c>
       <c r="F10" s="7">
-        <v>43738</v>
+        <v>43747</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="G10" s="7">
+        <v>43747</v>
+      </c>
+      <c r="H10" s="7">
+        <v>43747</v>
+      </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -856,18 +1043,26 @@
       <c r="V10" s="8"/>
       <c r="W10" s="8"/>
     </row>
-    <row r="11" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" s="16" customFormat="1" ht="247.5" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D11" s="10"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="E11" s="7">
+        <v>43747</v>
+      </c>
+      <c r="F11" s="7">
+        <v>43747</v>
+      </c>
+      <c r="G11" s="7">
+        <v>43747</v>
+      </c>
+      <c r="H11" s="7">
+        <v>43747</v>
+      </c>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
@@ -885,13 +1080,12 @@
       <c r="W11" s="8"/>
     </row>
     <row r="12" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10" t="s">
+      <c r="A12" s="16" t="s">
         <v>14</v>
       </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -913,11 +1107,21 @@
       <c r="W12" s="8"/>
     </row>
     <row r="13" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="B13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="7">
+        <v>43728</v>
+      </c>
+      <c r="F13" s="7">
+        <v>43738</v>
+      </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="8"/>
@@ -937,8 +1141,12 @@
       <c r="W13" s="8"/>
     </row>
     <row r="14" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
+      <c r="B14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="D14" s="10"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -961,9 +1169,13 @@
       <c r="W14" s="8"/>
     </row>
     <row r="15" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
+      <c r="B15" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
+      <c r="D15" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -1248,67 +1460,79 @@
       <c r="V26" s="8"/>
       <c r="W26" s="8"/>
     </row>
-    <row r="27" spans="2:23" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-    </row>
-    <row r="28" spans="2:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="1"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-    </row>
-    <row r="29" spans="2:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="1"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="13"/>
-      <c r="R29" s="13"/>
-      <c r="S29" s="13"/>
-    </row>
-    <row r="30" spans="2:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="9"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="8"/>
+      <c r="U27" s="8"/>
+      <c r="V27" s="8"/>
+      <c r="W27" s="8"/>
+    </row>
+    <row r="28" spans="2:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="9"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
+      <c r="T28" s="8"/>
+      <c r="U28" s="8"/>
+      <c r="V28" s="8"/>
+      <c r="W28" s="8"/>
+    </row>
+    <row r="29" spans="2:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="9"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="8"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="8"/>
+    </row>
+    <row r="30" spans="2:23" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
@@ -1335,7 +1559,7 @@
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
+      <c r="H31" s="14"/>
       <c r="I31" s="13"/>
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
@@ -20748,6 +20972,66 @@
       <c r="R1001" s="13"/>
       <c r="S1001" s="13"/>
     </row>
+    <row r="1002" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1002" s="1"/>
+      <c r="C1002" s="11"/>
+      <c r="D1002" s="11"/>
+      <c r="E1002" s="12"/>
+      <c r="F1002" s="12"/>
+      <c r="G1002" s="12"/>
+      <c r="H1002" s="12"/>
+      <c r="I1002" s="13"/>
+      <c r="J1002" s="13"/>
+      <c r="K1002" s="13"/>
+      <c r="L1002" s="13"/>
+      <c r="M1002" s="13"/>
+      <c r="N1002" s="13"/>
+      <c r="O1002" s="13"/>
+      <c r="P1002" s="13"/>
+      <c r="Q1002" s="13"/>
+      <c r="R1002" s="13"/>
+      <c r="S1002" s="13"/>
+    </row>
+    <row r="1003" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1003" s="1"/>
+      <c r="C1003" s="11"/>
+      <c r="D1003" s="11"/>
+      <c r="E1003" s="12"/>
+      <c r="F1003" s="12"/>
+      <c r="G1003" s="12"/>
+      <c r="H1003" s="12"/>
+      <c r="I1003" s="13"/>
+      <c r="J1003" s="13"/>
+      <c r="K1003" s="13"/>
+      <c r="L1003" s="13"/>
+      <c r="M1003" s="13"/>
+      <c r="N1003" s="13"/>
+      <c r="O1003" s="13"/>
+      <c r="P1003" s="13"/>
+      <c r="Q1003" s="13"/>
+      <c r="R1003" s="13"/>
+      <c r="S1003" s="13"/>
+    </row>
+    <row r="1004" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1004" s="1"/>
+      <c r="C1004" s="11"/>
+      <c r="D1004" s="11"/>
+      <c r="E1004" s="12"/>
+      <c r="F1004" s="12"/>
+      <c r="G1004" s="12"/>
+      <c r="H1004" s="12"/>
+      <c r="I1004" s="13"/>
+      <c r="J1004" s="13"/>
+      <c r="K1004" s="13"/>
+      <c r="L1004" s="13"/>
+      <c r="M1004" s="13"/>
+      <c r="N1004" s="13"/>
+      <c r="O1004" s="13"/>
+      <c r="P1004" s="13"/>
+      <c r="Q1004" s="13"/>
+      <c r="R1004" s="13"/>
+      <c r="S1004" s="13"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
@@ -20755,5 +21039,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>